<commit_message>
Updating diary entries up to 2.19.2020
</commit_message>
<xml_diff>
--- a/diaries/diary-HyunYang.xlsx
+++ b/diaries/diary-HyunYang.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hyun\IdeaProjects\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C35D44-C5BA-4674-BF4A-BCB9A143CA37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E74696-E55B-42C1-9346-0755647BE153}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="81">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -187,6 +187,93 @@
   </si>
   <si>
     <t>Overall I felt pretty accomplished and good about the amount of work we were able to do in the given time. Now that we've gone through the code numerous times, it felt much easier to sift through the code and identify the important features.</t>
+  </si>
+  <si>
+    <t>2.6.2020</t>
+  </si>
+  <si>
+    <t>Briefly Talk about Exam + Guest speaker</t>
+  </si>
+  <si>
+    <t>Learned what it means to be a developer in a smaller company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It made me really think about what it would be like to work at a small company as opposed to some place like Blizzard. It's very cool to see how much creative freedom someone in that position can have. </t>
+  </si>
+  <si>
+    <t>I felt small, thinking that there are so many options and choices we can make even under the same umbrella of "software engineer". I'm not quite sure if I would necessaryily like it better, but it's definitely something to think about.</t>
+  </si>
+  <si>
+    <t>2.13.2020</t>
+  </si>
+  <si>
+    <t>Exam day</t>
+  </si>
+  <si>
+    <t>Finished the exam! Whoot whoot. Also learned about  different stakeholders and what impact they may have on software development.</t>
+  </si>
+  <si>
+    <t>I've never really thought much about stakeholders other than the developer and the person who provides the requirements. It made me really think about, for example, in game development, how much the players really contribute to the game development, along with the investors who can really stear the direction of development.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I really hope that the people who invest in my work could give me a sense of creative freedom….I am not particularly fond of people who restrict me and throw money at me saying they get to decide…but then again it probably is how the world realistically works. </t>
+  </si>
+  <si>
+    <t>2.15.2020</t>
+  </si>
+  <si>
+    <t>2:00 - 7:00</t>
+  </si>
+  <si>
+    <t>Find Essential Feature (re-do)</t>
+  </si>
+  <si>
+    <t>Found our 2nd re-do essential feature (map generation). Wrote out outline of what we would write once we confirm with Kaj</t>
+  </si>
+  <si>
+    <t>We feel like we have a much clearer understanding as a group as to what an essential feature actually is. Before we considered what users may REALLY want, but that's different from a core part of the code that may break if it does not exist in the program</t>
+  </si>
+  <si>
+    <t>While it was initially frustrating to see how poorly we did on the assignment, it was refreshing to feel like we fully understood the concepts now, and hopefully don't run into such problems in the future.</t>
+  </si>
+  <si>
+    <t>2.18.2020</t>
+  </si>
+  <si>
+    <t>Nic, Rafael, Chris, Kaj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting with Kaj </t>
+  </si>
+  <si>
+    <t>3:45 - 4:30</t>
+  </si>
+  <si>
+    <t>Going over resubmission</t>
+  </si>
+  <si>
+    <t>It seems like we were on the right track, and we just needed to refine our writing and thought process. We also were going too low-level, and made it hard for the reader to really understand things at a high-level.</t>
+  </si>
+  <si>
+    <t>It felt good to be reassured that we weren't completely off the right track. It seems like Kaj is grading us….not harshly, but very realistically, which probably most people aren't used to. Even at an academic/university level. I hope that this version of our resubmission is much easier to understand.</t>
+  </si>
+  <si>
+    <t>2.19.2020</t>
+  </si>
+  <si>
+    <t>2:30 - 5:00</t>
+  </si>
+  <si>
+    <t>Complete Resubmission</t>
+  </si>
+  <si>
+    <t>Finished rewriting our first essential feature to be more legible and redid 2nd feature entirely.</t>
+  </si>
+  <si>
+    <t>It was good that we ended up meeting as a group rather than working independently. We regrouped every 10 minutes to make sure we were all on the same page, and rubber-duckied back and forth with what we planned on doing.</t>
+  </si>
+  <si>
+    <t>I feel great with our new submission. It feels complete, much more legible than our pervious iteration, and showcases a much higher-level understanding of the code rather than a lower-level repeat of code.</t>
   </si>
 </sst>
 </file>
@@ -331,7 +418,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -361,9 +448,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="4" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -378,6 +462,12 @@
     </xf>
     <xf numFmtId="18" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -699,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="57" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="57" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,24 +799,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -818,516 +908,586 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="12">
+      <c r="A10" s="11">
         <v>43839</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="13">
         <v>0.29166666666666669</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="12">
+      <c r="A11" s="11">
         <v>43846</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="14" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="12">
+      <c r="A12" s="11">
         <v>43848</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="15">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="12">
+      <c r="A13" s="11">
         <v>43853</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="171.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="12">
+      <c r="A14" s="11">
         <v>43855</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="78" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="14" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="156" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="8"/>
+    <row r="17" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="156" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="156" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="8"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="17"/>
     </row>
     <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="8"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="17"/>
     </row>
     <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="8"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="17"/>
     </row>
     <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="8"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="17"/>
     </row>
     <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="8"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="17"/>
     </row>
     <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="8"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="17"/>
     </row>
     <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="8"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="17"/>
     </row>
     <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="8"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="17"/>
     </row>
     <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="8"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="17"/>
     </row>
     <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="8"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="17"/>
     </row>
     <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="8"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="17"/>
     </row>
     <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="8"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="17"/>
     </row>
     <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="8"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="17"/>
     </row>
     <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="8"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="8"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="17"/>
     </row>
     <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="8"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="17"/>
     </row>
     <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="8"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="17"/>
     </row>
     <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="8"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="17"/>
     </row>
     <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="8"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="8"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="8"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="8"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="17"/>
     </row>
     <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="8"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="17"/>
     </row>
     <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="8"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="17"/>
     </row>
     <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="8"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="17"/>
     </row>
     <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="8"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="8"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="8"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="8"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="17"/>
     </row>
     <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="8"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="17"/>
     </row>
     <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="8"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="17"/>
     </row>
     <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="8"/>
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="17"/>
     </row>
     <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="8"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="7"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="8"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="7"/>

</xml_diff>